<commit_message>
tweaked the film popover to width of 225 - pfv
</commit_message>
<xml_diff>
--- a/public/films2.xlsx
+++ b/public/films2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>title</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>dvd_wstock</t>
+  </si>
+  <si>
+    <t>a good film</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="D7" sqref="D7:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,6 +887,9 @@
       <c r="C7">
         <v>2007</v>
       </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -925,6 +931,9 @@
       <c r="C8">
         <v>2013</v>
       </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
@@ -966,6 +975,9 @@
       <c r="C9">
         <v>1984</v>
       </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
@@ -1007,6 +1019,9 @@
       <c r="C10">
         <v>2011</v>
       </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
@@ -1048,6 +1063,9 @@
       <c r="C11">
         <v>2011</v>
       </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
@@ -1088,6 +1106,9 @@
       </c>
       <c r="C12">
         <v>2013</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>

</xml_diff>